<commit_message>
fixed tests, added import of all cells
</commit_message>
<xml_diff>
--- a/tests/Formatting Test File.xlsx
+++ b/tests/Formatting Test File.xlsx
@@ -44,6 +44,7 @@
       <color rgb="FF000000"/>
       <name val="나눔고딕"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -106,7 +107,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,8 +120,14 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBA131A"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -205,6 +212,13 @@
       <bottom style="medium"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -233,12 +247,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -254,7 +268,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -274,7 +288,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -286,7 +300,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -302,7 +316,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -322,7 +336,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -330,11 +344,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -342,12 +356,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -363,6 +381,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFBA131A"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -371,10 +449,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K23"/>
+  <dimension ref="A2:K26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -533,10 +611,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="29" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="29"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G17" s="29"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="29"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="29"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="29"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="29"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="29"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="30" t="s">
         <v>1</v>
       </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="29"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="29"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fix: store reference to the worksheet and value if there is any
</commit_message>
<xml_diff>
--- a/tests/Formatting Test File.xlsx
+++ b/tests/Formatting Test File.xlsx
@@ -20,9 +20,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t xml:space="preserve">B3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B14</t>
+  </si>
   <si>
     <t xml:space="preserve">excel diagnostic test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K14</t>
   </si>
   <si>
     <t xml:space="preserve">ABC</t>
@@ -272,7 +308,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -292,7 +328,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -304,7 +340,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -324,7 +360,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -452,7 +488,7 @@
   <dimension ref="A2:K26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
+      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -481,13 +517,18 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="K3" s="0" t="str">
         <f aca="false">$A$23</f>
         <v>ABC</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="C4" s="7"/>
       <c r="D4" s="8"/>
       <c r="F4" s="9" t="str">
@@ -500,7 +541,9 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="11"/>
+      <c r="B5" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="12"/>
       <c r="I5" s="13" t="n">
@@ -514,7 +557,9 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="14"/>
+      <c r="B6" s="14" t="s">
+        <v>3</v>
+      </c>
       <c r="C6" s="15"/>
       <c r="D6" s="16"/>
       <c r="I6" s="13"/>
@@ -525,6 +570,9 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>4</v>
+      </c>
       <c r="F7" s="18" t="str">
         <f aca="false">$A$23</f>
         <v>ABC</v>
@@ -535,7 +583,9 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="19"/>
+      <c r="B8" s="19" t="s">
+        <v>5</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="20"/>
       <c r="F8" s="0" t="str">
@@ -553,6 +603,9 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
       <c r="F9" s="23" t="str">
         <f aca="false">$A$23</f>
         <v>ABC</v>
@@ -563,7 +616,9 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12"/>
+      <c r="B10" s="12" t="s">
+        <v>7</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="F10" s="0" t="str">
         <f aca="false">$A$23</f>
@@ -579,6 +634,9 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="F11" s="26" t="str">
         <f aca="false">$A$23</f>
         <v>ABC</v>
@@ -593,6 +651,9 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>9</v>
+      </c>
       <c r="K12" s="5" t="str">
         <f aca="false">$A$23</f>
         <v>ABC</v>
@@ -606,9 +667,15 @@
       <c r="C13" s="27"/>
       <c r="D13" s="27"/>
     </row>
-    <row r="14" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>10</v>
+      </c>
       <c r="F14" s="28" t="s">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -634,7 +701,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="30" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C23" s="29"/>
       <c r="D23" s="29"/>

</xml_diff>